<commit_message>
Added more languages using Google Translate
</commit_message>
<xml_diff>
--- a/Histamin_DEU.xlsx
+++ b/Histamin_DEU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\histamin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\histamin\histamin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4FF0EE-3245-4937-A43B-C0AF764DB9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8C0246-867F-4240-ABA5-05255C211FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{C73EBCAD-1997-423D-8B6C-85F5CF94A929}"/>
   </bookViews>
@@ -3549,7 +3549,7 @@
     <t>Rasche Histaminbildung</t>
   </si>
   <si>
-    <t>Ingredient</t>
+    <t>Zutat</t>
   </si>
 </sst>
 </file>
@@ -4292,7 +4292,7 @@
     <tableColumn id="4" xr3:uid="{C6A4403B-2B22-4884-AEAC-292D11162007}" name="Andere Amine" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{C556507B-4CAF-4F25-BDB5-03819C5B61BE}" name="Liberator" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{15FAB530-8B54-4271-B2C6-3F7D504CFBF4}" name="Blocker" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{098A10BB-39FC-4C4B-A5D1-D744FA8DEEA4}" name="Ingredient" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{098A10BB-39FC-4C4B-A5D1-D744FA8DEEA4}" name="Zutat" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{6A5A93CB-0F75-4D08-90FC-09F6C2890270}" name="Anmerkungen" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{86E5DE20-B7AF-438A-96C0-A886E5D092ED}" name="Kategorie" dataDxfId="1"/>
   </tableColumns>
@@ -4622,7 +4622,7 @@
   <dimension ref="A1:I963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -22897,6 +22897,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010067FB9B2906952545AF079B434A2EE536" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="65b6317d776d0ca9c56e393355e1d2e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d507d695-0644-46d1-a3c4-b2b314b1e71b" xmlns:ns4="465add03-947d-4036-9a17-2f228d102e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="77ed74fa905ec2d918ef59a67a552ed2" ns3:_="" ns4:_="">
     <xsd:import namespace="d507d695-0644-46d1-a3c4-b2b314b1e71b"/>
@@ -23125,15 +23134,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4456688A-E9C4-44AF-B0E2-77CE491D18A5}">
   <ds:schemaRefs>
@@ -23152,6 +23152,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{450EF11D-D081-4A84-90AC-F214A618AC7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4158F68B-5494-4396-93C3-EA848C06F329}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23168,12 +23176,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{450EF11D-D081-4A84-90AC-F214A618AC7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>